<commit_message>
thêm tính năng mức độ câu hỏi ở trong file excel
</commit_message>
<xml_diff>
--- a/public/upload/files/mau-them-danh-sach-Questions.xlsx
+++ b/public/upload/files/mau-them-danh-sach-Questions.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DUC BA\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\thionline\public\upload\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <r>
       <t>Lưu ý:</t>
@@ -195,6 +195,33 @@
         <family val="2"/>
       </rPr>
       <t xml:space="preserve"> không cần phải nhập </t>
+    </r>
+  </si>
+  <si>
+    <t>muc_do_cau_hoi</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Cột </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>muc_do_cau_hoi</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> yêu cầu phải nhập đúng như trong hệ thống đã ghi để tránh bị lỗi khi nhập vào</t>
     </r>
   </si>
 </sst>
@@ -275,6 +302,14 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -284,14 +319,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -605,37 +632,37 @@
   <dimension ref="A1:N9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:N3"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="6.5703125" customWidth="1"/>
     <col min="2" max="2" width="37.42578125" customWidth="1"/>
-    <col min="3" max="3" width="34.7109375" customWidth="1"/>
-    <col min="4" max="4" width="33" customWidth="1"/>
-    <col min="5" max="5" width="36.7109375" customWidth="1"/>
-    <col min="6" max="6" width="39.5703125" style="3" customWidth="1"/>
-    <col min="7" max="7" width="10.5703125" style="5" customWidth="1"/>
+    <col min="3" max="3" width="32.7109375" customWidth="1"/>
+    <col min="4" max="4" width="28" customWidth="1"/>
+    <col min="5" max="5" width="27" customWidth="1"/>
+    <col min="6" max="6" width="33.85546875" style="3" customWidth="1"/>
+    <col min="7" max="7" width="16.42578125" style="5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="20.25" x14ac:dyDescent="0.3">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="12"/>
-      <c r="C1" s="12"/>
-      <c r="D1" s="12"/>
-      <c r="E1" s="12"/>
-      <c r="F1" s="12"/>
-      <c r="G1" s="13"/>
-      <c r="H1" s="13"/>
-      <c r="I1" s="13"/>
-      <c r="J1" s="13"/>
-      <c r="K1" s="13"/>
-      <c r="L1" s="13"/>
-      <c r="M1" s="13"/>
-      <c r="N1" s="13"/>
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
+      <c r="F1" s="10"/>
+      <c r="G1" s="8"/>
+      <c r="H1" s="8"/>
+      <c r="I1" s="8"/>
+      <c r="J1" s="8"/>
+      <c r="K1" s="8"/>
+      <c r="L1" s="8"/>
+      <c r="M1" s="8"/>
+      <c r="N1" s="8"/>
     </row>
     <row r="2" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="11" t="s">
@@ -646,60 +673,62 @@
       <c r="D2" s="11"/>
       <c r="E2" s="11"/>
       <c r="F2" s="11"/>
-      <c r="G2" s="14"/>
-      <c r="H2" s="14"/>
-      <c r="I2" s="14"/>
-      <c r="J2" s="14"/>
-      <c r="K2" s="14"/>
-      <c r="L2" s="14"/>
-      <c r="M2" s="14"/>
-      <c r="N2" s="14"/>
+      <c r="G2" s="9"/>
+      <c r="H2" s="9"/>
+      <c r="I2" s="9"/>
+      <c r="J2" s="9"/>
+      <c r="K2" s="9"/>
+      <c r="L2" s="9"/>
+      <c r="M2" s="9"/>
+      <c r="N2" s="9"/>
     </row>
     <row r="3" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="9" t="s">
+      <c r="A3" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="9"/>
-      <c r="C3" s="9"/>
-      <c r="D3" s="9"/>
-      <c r="E3" s="9"/>
-      <c r="F3" s="9"/>
-      <c r="G3" s="9"/>
-      <c r="H3" s="9"/>
-      <c r="I3" s="9"/>
-      <c r="J3" s="9"/>
-      <c r="K3" s="9"/>
-      <c r="L3" s="9"/>
-      <c r="M3" s="9"/>
-      <c r="N3" s="9"/>
+      <c r="B3" s="13"/>
+      <c r="C3" s="13"/>
+      <c r="D3" s="13"/>
+      <c r="E3" s="13"/>
+      <c r="F3" s="13"/>
+      <c r="G3" s="13"/>
+      <c r="H3" s="13"/>
+      <c r="I3" s="13"/>
+      <c r="J3" s="13"/>
+      <c r="K3" s="13"/>
+      <c r="L3" s="13"/>
+      <c r="M3" s="13"/>
+      <c r="N3" s="13"/>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A4" s="10"/>
-      <c r="B4" s="10"/>
-      <c r="C4" s="10"/>
-      <c r="D4" s="10"/>
-      <c r="E4" s="10"/>
-      <c r="F4" s="10"/>
-      <c r="G4" s="10"/>
-      <c r="H4" s="10"/>
-      <c r="I4" s="10"/>
-      <c r="J4" s="10"/>
-      <c r="K4" s="10"/>
-      <c r="L4" s="10"/>
-      <c r="M4" s="10"/>
-      <c r="N4" s="10"/>
+      <c r="A4" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="14"/>
+      <c r="C4" s="14"/>
+      <c r="D4" s="14"/>
+      <c r="E4" s="14"/>
+      <c r="F4" s="14"/>
+      <c r="G4" s="14"/>
+      <c r="H4" s="14"/>
+      <c r="I4" s="14"/>
+      <c r="J4" s="14"/>
+      <c r="K4" s="14"/>
+      <c r="L4" s="14"/>
+      <c r="M4" s="14"/>
+      <c r="N4" s="14"/>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A5" s="10"/>
-      <c r="B5" s="10"/>
-      <c r="C5" s="10"/>
-      <c r="D5" s="10"/>
-      <c r="E5" s="10"/>
-      <c r="F5" s="10"/>
-      <c r="G5" s="10"/>
-      <c r="H5" s="10"/>
-      <c r="I5" s="10"/>
-      <c r="J5" s="10"/>
+      <c r="A5" s="14"/>
+      <c r="B5" s="14"/>
+      <c r="C5" s="14"/>
+      <c r="D5" s="14"/>
+      <c r="E5" s="14"/>
+      <c r="F5" s="14"/>
+      <c r="G5" s="14"/>
+      <c r="H5" s="14"/>
+      <c r="I5" s="14"/>
+      <c r="J5" s="14"/>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
@@ -720,7 +749,9 @@
       <c r="F6" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="G6" s="6"/>
+      <c r="G6" s="6" t="s">
+        <v>9</v>
+      </c>
       <c r="H6" s="2"/>
       <c r="I6" s="2"/>
       <c r="J6" s="2"/>
@@ -734,10 +765,10 @@
       <c r="H7" s="3"/>
       <c r="I7" s="3"/>
       <c r="J7" s="3"/>
-      <c r="K7" s="8"/>
-      <c r="L7" s="8"/>
-      <c r="M7" s="8"/>
-      <c r="N7" s="8"/>
+      <c r="K7" s="12"/>
+      <c r="L7" s="12"/>
+      <c r="M7" s="12"/>
+      <c r="N7" s="12"/>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A8">
@@ -747,20 +778,20 @@
       <c r="H8" s="3"/>
       <c r="I8" s="3"/>
       <c r="J8" s="3"/>
-      <c r="K8" s="8"/>
-      <c r="L8" s="8"/>
-      <c r="M8" s="8"/>
-      <c r="N8" s="8"/>
+      <c r="K8" s="12"/>
+      <c r="L8" s="12"/>
+      <c r="M8" s="12"/>
+      <c r="N8" s="12"/>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.2">
       <c r="D9" s="7"/>
       <c r="H9" s="3"/>
       <c r="I9" s="3"/>
       <c r="J9" s="3"/>
-      <c r="K9" s="8"/>
-      <c r="L9" s="8"/>
-      <c r="M9" s="8"/>
-      <c r="N9" s="8"/>
+      <c r="K9" s="12"/>
+      <c r="L9" s="12"/>
+      <c r="M9" s="12"/>
+      <c r="N9" s="12"/>
     </row>
   </sheetData>
   <mergeCells count="8">

</xml_diff>